<commit_message>
capital sheet to balance sheet
</commit_message>
<xml_diff>
--- a/data/data_patch.xlsx
+++ b/data/data_patch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\trading_plan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37A062D-E6C9-4B38-8121-8BFC79FA3897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B020B9-C6DE-4E14-98E4-30DBBEBF6CD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16170" yWindow="16050" windowWidth="16200" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capital" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>2_m_sw_9790</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,43 +87,51 @@
     <t>AcctIDByMXZ</t>
   </si>
   <si>
-    <t>NetAsset</t>
+    <t>Symbol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShortQty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CashEquivalent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompositeLongAmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ApproximateNetAsset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETFLongAmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETFShortAmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompositeShortAmt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TotalAsset</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TotalLiability</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>928_m_zx_6258</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Symbol</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShortQty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cash</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CashEquivalent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LongAmt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Note</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -450,59 +458,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2014A2-72F2-459D-8409-EBB38C0BE405}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>13278795</v>
-      </c>
-      <c r="C2">
-        <v>19009900</v>
-      </c>
-      <c r="D2">
-        <v>5731104</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -541,19 +546,19 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update sec debt algorithm
</commit_message>
<xml_diff>
--- a/data/data_patch.xlsx
+++ b/data/data_patch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\trading_plan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C25E33D-A55D-4D64-A83E-9AA1982F2A82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B81700-F4B4-405C-912C-8FCDC15B926B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14955" yWindow="6615" windowWidth="14205" windowHeight="17250" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capital" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>2_m_sw_9790</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>UnderlyingStartValue_vec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiabilityStartValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InterestRate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DatedDate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -599,10 +611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -614,15 +626,18 @@
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -645,25 +660,34 @@
         <v>32</v>
       </c>
       <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +710,7 @@
         <v>-23031910</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -709,7 +733,7 @@
         <v>-60614206</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -732,7 +756,7 @@
         <v>-27117532</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -755,7 +779,7 @@
         <v>-98809529.790000007</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -778,7 +802,7 @@
         <v>-19247136.489999998</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -801,7 +825,7 @@
         <v>-30853356.800000001</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -823,19 +847,19 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L8" t="s">
         <v>3</v>
       </c>
-      <c r="J8" t="s">
+      <c r="M8" t="s">
         <v>29</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>-2674.7550000000001</v>
       </c>
-      <c r="L8">
+      <c r="O8">
         <v>-15000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
product series 9,7,12 database updated.
</commit_message>
<xml_diff>
--- a/data/data_patch.xlsx
+++ b/data/data_patch.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\trading_plan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0700525E-6C1F-4A4F-B5F7-7F0CE6384066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C7359D-8CC7-4DC9-8874-2B1B4956061A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14955" yWindow="6615" windowWidth="14205" windowHeight="17250" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1995" yWindow="3900" windowWidth="14205" windowHeight="17250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capital" sheetId="2" r:id="rId1"/>
     <sheet name="holding" sheetId="1" r:id="rId2"/>
-    <sheet name="temp" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>2_m_sw_9790</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,6 +216,10 @@
   </si>
   <si>
     <t>20200615</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>707_m_zxjt_2313</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -263,10 +266,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -547,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2014A2-72F2-459D-8409-EBB38C0BE405}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -619,6 +623,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5000000</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -629,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -967,19 +979,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EFE95A-AF69-412C-84C2-B08BB41E5287}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>